<commit_message>
Fixed issue in cleaning data functions
</commit_message>
<xml_diff>
--- a/build_datasets/Data/non_mlb_data/Ballpark Info.xlsx
+++ b/build_datasets/Data/non_mlb_data/Ballpark Info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaredzirkes/Desktop/Python/GitHub/Project - MLB Simulation/Outside Info Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaredzirkes/Desktop/Python/GitHub/mlb_simulation/build_datasets/Data/non_mlb_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8173374E-EAF7-B34D-85A6-774455EE16E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC93638-FD07-0646-8DD0-6845310BC6CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36600" yWindow="1380" windowWidth="28800" windowHeight="16420" xr2:uid="{DD70C302-6D58-ED4E-8908-4F905B2811BD}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16500" xr2:uid="{DD70C302-6D58-ED4E-8908-4F905B2811BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -594,7 +594,7 @@
   <dimension ref="C3:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
finished base simulation code
</commit_message>
<xml_diff>
--- a/build_datasets/Data/non_mlb_data/Ballpark Info.xlsx
+++ b/build_datasets/Data/non_mlb_data/Ballpark Info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaredzirkes/Desktop/Python/GitHub/mlb_simulation/build_datasets/Data/non_mlb_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaredzirkes/Desktop/Python/projects/mlb_simulation/build_datasets/data/non_mlb_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC93638-FD07-0646-8DD0-6845310BC6CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB92AB18-F47A-8141-BCC0-EBACEB711E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16500" xr2:uid="{DD70C302-6D58-ED4E-8908-4F905B2811BD}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="16500" xr2:uid="{DD70C302-6D58-ED4E-8908-4F905B2811BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="98">
   <si>
     <t>Stadium</t>
   </si>
@@ -240,6 +240,96 @@
   </si>
   <si>
     <t>ARI</t>
+  </si>
+  <si>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>Red Sox</t>
+  </si>
+  <si>
+    <t>Cubs</t>
+  </si>
+  <si>
+    <t>Dodgers</t>
+  </si>
+  <si>
+    <t>Athletics</t>
+  </si>
+  <si>
+    <t>Angels</t>
+  </si>
+  <si>
+    <t>Royals</t>
+  </si>
+  <si>
+    <t>Blue Jays</t>
+  </si>
+  <si>
+    <t>Rays</t>
+  </si>
+  <si>
+    <t>White Sox</t>
+  </si>
+  <si>
+    <t>Orioles</t>
+  </si>
+  <si>
+    <t>Guardians</t>
+  </si>
+  <si>
+    <t>Rockies</t>
+  </si>
+  <si>
+    <t>Diamondbacks</t>
+  </si>
+  <si>
+    <t>Mariners</t>
+  </si>
+  <si>
+    <t>Giants</t>
+  </si>
+  <si>
+    <t>Astros</t>
+  </si>
+  <si>
+    <t>Tigers</t>
+  </si>
+  <si>
+    <t>Pirates</t>
+  </si>
+  <si>
+    <t>Brewers</t>
+  </si>
+  <si>
+    <t>Reds</t>
+  </si>
+  <si>
+    <t>Padres</t>
+  </si>
+  <si>
+    <t>Phillies</t>
+  </si>
+  <si>
+    <t>Cardinals</t>
+  </si>
+  <si>
+    <t>Yankees</t>
+  </si>
+  <si>
+    <t>Mets</t>
+  </si>
+  <si>
+    <t>Twins</t>
+  </si>
+  <si>
+    <t>Marlins</t>
+  </si>
+  <si>
+    <t>Braves</t>
+  </si>
+  <si>
+    <t>Rangers</t>
   </si>
 </sst>
 </file>
@@ -255,12 +345,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -275,8 +371,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,15 +688,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E93A338-5212-F54C-A80A-896B308BCAC7}">
-  <dimension ref="C3:F38"/>
+  <dimension ref="C3:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>0</v>
       </c>
@@ -612,8 +709,11 @@
       <c r="F3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>2</v>
       </c>
@@ -624,10 +724,13 @@
         <v>1900</v>
       </c>
       <c r="F4">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.2">
+        <v>2026</v>
+      </c>
+      <c r="G4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>3</v>
       </c>
@@ -638,10 +741,13 @@
         <v>1900</v>
       </c>
       <c r="F5">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.2">
+        <v>2026</v>
+      </c>
+      <c r="G5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>4</v>
       </c>
@@ -652,24 +758,30 @@
         <v>1900</v>
       </c>
       <c r="F6">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C7" t="s">
+        <v>2026</v>
+      </c>
+      <c r="G6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E7">
-        <v>1900</v>
-      </c>
-      <c r="F7">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="E7" s="1">
+        <v>1900</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2026</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
         <v>6</v>
       </c>
@@ -680,10 +792,13 @@
         <v>1900</v>
       </c>
       <c r="F8">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.2">
+        <v>2026</v>
+      </c>
+      <c r="G8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
         <v>7</v>
       </c>
@@ -694,10 +809,13 @@
         <v>1900</v>
       </c>
       <c r="F9">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.2">
+        <v>2026</v>
+      </c>
+      <c r="G9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
         <v>8</v>
       </c>
@@ -708,10 +826,13 @@
         <v>1900</v>
       </c>
       <c r="F10">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.2">
+        <v>2020</v>
+      </c>
+      <c r="G10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
         <v>9</v>
       </c>
@@ -722,10 +843,13 @@
         <v>1900</v>
       </c>
       <c r="F11">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.2">
+        <v>2026</v>
+      </c>
+      <c r="G11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
         <v>10</v>
       </c>
@@ -736,10 +860,13 @@
         <v>1900</v>
       </c>
       <c r="F12">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.2">
+        <v>2026</v>
+      </c>
+      <c r="G12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
         <v>11</v>
       </c>
@@ -750,10 +877,13 @@
         <v>1900</v>
       </c>
       <c r="F13">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.2">
+        <v>2026</v>
+      </c>
+      <c r="G13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
         <v>12</v>
       </c>
@@ -764,10 +894,13 @@
         <v>1900</v>
       </c>
       <c r="F14">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="15" spans="3:6" x14ac:dyDescent="0.2">
+        <v>2026</v>
+      </c>
+      <c r="G14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
         <v>13</v>
       </c>
@@ -778,10 +911,13 @@
         <v>1900</v>
       </c>
       <c r="F15">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="16" spans="3:6" x14ac:dyDescent="0.2">
+        <v>2026</v>
+      </c>
+      <c r="G15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
         <v>14</v>
       </c>
@@ -792,10 +928,13 @@
         <v>1900</v>
       </c>
       <c r="F16">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.2">
+        <v>2026</v>
+      </c>
+      <c r="G16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
         <v>14</v>
       </c>
@@ -806,10 +945,13 @@
         <v>1900</v>
       </c>
       <c r="F17">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.2">
+        <v>2026</v>
+      </c>
+      <c r="G17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
         <v>15</v>
       </c>
@@ -820,10 +962,13 @@
         <v>1900</v>
       </c>
       <c r="F18">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.2">
+        <v>2026</v>
+      </c>
+      <c r="G18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
         <v>16</v>
       </c>
@@ -834,10 +979,13 @@
         <v>1900</v>
       </c>
       <c r="F19">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.2">
+        <v>2026</v>
+      </c>
+      <c r="G19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
         <v>17</v>
       </c>
@@ -848,10 +996,13 @@
         <v>1900</v>
       </c>
       <c r="F20">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.2">
+        <v>2026</v>
+      </c>
+      <c r="G20" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
         <v>18</v>
       </c>
@@ -862,10 +1013,13 @@
         <v>1900</v>
       </c>
       <c r="F21">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.2">
+        <v>2026</v>
+      </c>
+      <c r="G21" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
         <v>19</v>
       </c>
@@ -876,10 +1030,13 @@
         <v>1900</v>
       </c>
       <c r="F22">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.2">
+        <v>2026</v>
+      </c>
+      <c r="G22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
         <v>20</v>
       </c>
@@ -890,10 +1047,13 @@
         <v>1900</v>
       </c>
       <c r="F23">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.2">
+        <v>2026</v>
+      </c>
+      <c r="G23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
         <v>21</v>
       </c>
@@ -904,10 +1064,13 @@
         <v>1900</v>
       </c>
       <c r="F24">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.2">
+        <v>2026</v>
+      </c>
+      <c r="G24" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
         <v>22</v>
       </c>
@@ -918,10 +1081,13 @@
         <v>1900</v>
       </c>
       <c r="F25">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.2">
+        <v>2026</v>
+      </c>
+      <c r="G25" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
         <v>23</v>
       </c>
@@ -932,10 +1098,13 @@
         <v>1900</v>
       </c>
       <c r="F26">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.2">
+        <v>2026</v>
+      </c>
+      <c r="G26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
         <v>24</v>
       </c>
@@ -946,10 +1115,13 @@
         <v>1900</v>
       </c>
       <c r="F27">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.2">
+        <v>2026</v>
+      </c>
+      <c r="G27" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
         <v>25</v>
       </c>
@@ -960,10 +1132,13 @@
         <v>1900</v>
       </c>
       <c r="F28">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.2">
+        <v>2026</v>
+      </c>
+      <c r="G28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
         <v>26</v>
       </c>
@@ -974,10 +1149,13 @@
         <v>1900</v>
       </c>
       <c r="F29">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.2">
+        <v>2026</v>
+      </c>
+      <c r="G29" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
         <v>64</v>
       </c>
@@ -988,10 +1166,13 @@
         <v>1900</v>
       </c>
       <c r="F30">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.2">
+        <v>2026</v>
+      </c>
+      <c r="G30" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
         <v>27</v>
       </c>
@@ -1002,10 +1183,13 @@
         <v>1900</v>
       </c>
       <c r="F31">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.2">
+        <v>2026</v>
+      </c>
+      <c r="G31" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C32" t="s">
         <v>28</v>
       </c>
@@ -1016,10 +1200,13 @@
         <v>1900</v>
       </c>
       <c r="F32">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.2">
+        <v>2026</v>
+      </c>
+      <c r="G32" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C33" t="s">
         <v>30</v>
       </c>
@@ -1032,8 +1219,11 @@
       <c r="F33">
         <v>2016</v>
       </c>
-    </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="G33" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C34" t="s">
         <v>29</v>
       </c>
@@ -1044,10 +1234,13 @@
         <v>2017</v>
       </c>
       <c r="F34">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.2">
+        <v>2026</v>
+      </c>
+      <c r="G34" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C35" t="s">
         <v>62</v>
       </c>
@@ -1060,8 +1253,11 @@
       <c r="F35">
         <v>2019</v>
       </c>
-    </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="G35" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C36" t="s">
         <v>63</v>
       </c>
@@ -1072,10 +1268,13 @@
         <v>2020</v>
       </c>
       <c r="F36">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.2">
+        <v>2026</v>
+      </c>
+      <c r="G36" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C37" t="s">
         <v>66</v>
       </c>
@@ -1088,8 +1287,11 @@
       <c r="F37">
         <v>2021</v>
       </c>
-    </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="G37" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C38" t="s">
         <v>8</v>
       </c>
@@ -1101,6 +1303,9 @@
       </c>
       <c r="F38">
         <v>2024</v>
+      </c>
+      <c r="G38" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>